<commit_message>
add parsing to the model
</commit_message>
<xml_diff>
--- a/build/flutter_assets/assets/tags.xlsx
+++ b/build/flutter_assets/assets/tags.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HA\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HA Technology\excel_demo\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4FAACDF-9379-4426-9682-FFCDA56500AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FCD84DC1-E484-4A40-A6EB-64A67568F9C7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
   <si>
     <t>Address</t>
   </si>
@@ -69,9 +68,6 @@
     <t>DB1.DBX0.2</t>
   </si>
   <si>
-    <t>Description</t>
-  </si>
-  <si>
     <t>TagName</t>
   </si>
   <si>
@@ -85,12 +81,18 @@
   </si>
   <si>
     <t>500ms</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>description</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -470,11 +472,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35D34DBF-2861-4722-BC88-A19997B92E9F}">
-  <dimension ref="A1:F4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E5"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -486,9 +488,9 @@
     <col min="5" max="5" width="15.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -500,13 +502,16 @@
         <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F1" t="s">
-        <v>11</v>
+        <v>16</v>
+      </c>
+      <c r="G1" t="s">
+        <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:7">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -520,10 +525,13 @@
         <v>5</v>
       </c>
       <c r="E2" t="s">
-        <v>14</v>
+        <v>13</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:7">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -537,10 +545,13 @@
         <v>5</v>
       </c>
       <c r="E3" t="s">
-        <v>15</v>
+        <v>14</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:7">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -554,7 +565,10 @@
         <v>5</v>
       </c>
       <c r="E4" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>